<commit_message>
changes every (change for another)
</commit_message>
<xml_diff>
--- a/logs/registro_actividad_balanzas.xlsx
+++ b/logs/registro_actividad_balanzas.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F106"/>
+  <dimension ref="A1:F120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3367,6 +3367,245 @@
         </is>
       </c>
     </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2025-06-06 19:47:06</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Cierre Aplicacion</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Cerrado desde login.</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2025-06-06 19:47:13</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Cierre Aplicacion</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Cerrado desde login.</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2025-06-06 19:47:46</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Cierre Aplicacion</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Cerrado desde login.</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2025-06-06 19:47:57</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Cierre Aplicacion</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Cerrado desde login.</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2025-06-06 19:49:07</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Cierre Aplicacion</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Cerrado desde login.</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2025-06-06 19:49:18</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Cierre Aplicacion</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Cerrado desde login.</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2025-06-06 19:49:35</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Cierre Aplicacion</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Cerrado desde login.</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2025-06-06 19:49:52</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Cierre Aplicacion</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Cerrado desde login.</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2025-06-06 19:50:14</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Cierre Aplicacion</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Cerrado desde login.</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2025-06-06 19:53:19</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Cierre Aplicacion</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Cerrado desde login.</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2025-06-06 20:02:25</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Cierre Aplicacion</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Cerrado desde login.</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2025-06-06 20:02:26</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Cierre Aplicacion</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Cerrado desde login.</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2025-06-06 20:04:52</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Cierre Aplicacion</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Cerrado desde login.</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2025-06-06 20:08:23</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Cierre Aplicacion</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Cerrado desde login.</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>